<commit_message>
db and perf data added
</commit_message>
<xml_diff>
--- a/data/tmm_template.xlsx
+++ b/data/tmm_template.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tietoevry-my.sharepoint.com/personal/arun_loganathan_tietoevry_com/Documents/workspace/tmm_dashboard_streamlit_cloud/tmm_dashboard_app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{FAB75980-B740-0B40-A252-06969CBDD95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDC0EEF1-4B9C-3C4A-978A-4B23E030AC34}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{FAB75980-B740-0B40-A252-06969CBDD95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D472CE4-C284-CB47-992E-977BBCB2A2E7}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16940" activeTab="1" xr2:uid="{6FC6947F-CD69-5746-A992-4DF59BEE85A0}"/>
+    <workbookView xWindow="1720" yWindow="680" windowWidth="24460" windowHeight="16940" activeTab="3" xr2:uid="{6FC6947F-CD69-5746-A992-4DF59BEE85A0}"/>
   </bookViews>
   <sheets>
     <sheet name="QA PROCESS" sheetId="1" r:id="rId1"/>
-    <sheet name="AUTOMATION PROCESS" sheetId="2" r:id="rId2"/>
+    <sheet name="AUTOMATION TESTING" sheetId="2" r:id="rId2"/>
+    <sheet name="DATABASE TESTING" sheetId="3" r:id="rId3"/>
+    <sheet name="PERFORMANCE TESTING" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="186">
   <si>
     <t>CHECK</t>
   </si>
@@ -286,13 +288,322 @@
   </si>
   <si>
     <t>Build Integration process</t>
+  </si>
+  <si>
+    <t>Data Test Planning Analysis</t>
+  </si>
+  <si>
+    <t>Data Landscape Check</t>
+  </si>
+  <si>
+    <t>Automation Script/Tool Evaluation</t>
+  </si>
+  <si>
+    <t>Query log/Clarification log Updation</t>
+  </si>
+  <si>
+    <t>Data Profiling</t>
+  </si>
+  <si>
+    <t>Data Test Strategy Efficiency</t>
+  </si>
+  <si>
+    <t>Data Test Plan Efficiency</t>
+  </si>
+  <si>
+    <t>Test Environment Readiness</t>
+  </si>
+  <si>
+    <t>Test Data Management</t>
+  </si>
+  <si>
+    <t>Source Test Data Availability</t>
+  </si>
+  <si>
+    <t>TDM Tool Usage</t>
+  </si>
+  <si>
+    <t>Test Data Volume</t>
+  </si>
+  <si>
+    <t>Test Data (Positive &amp; Negative Scenarios)</t>
+  </si>
+  <si>
+    <t>Data Test Coverage</t>
+  </si>
+  <si>
+    <t>Initial Data test Coverage</t>
+  </si>
+  <si>
+    <t>Incremental Delta Coverage</t>
+  </si>
+  <si>
+    <t>File watcher Check</t>
+  </si>
+  <si>
+    <t>Inaccurate file/Data check</t>
+  </si>
+  <si>
+    <t>Source to Target transformation check</t>
+  </si>
+  <si>
+    <t>Reject Record Check</t>
+  </si>
+  <si>
+    <t>Duplication Check</t>
+  </si>
+  <si>
+    <t>Key Integrity Check</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SQL/HQL Efficiency</t>
+  </si>
+  <si>
+    <t>Query Optimization</t>
+  </si>
+  <si>
+    <t>Data Migration Check</t>
+  </si>
+  <si>
+    <t>Scheduler Check</t>
+  </si>
+  <si>
+    <t>Aggregate data Check</t>
+  </si>
+  <si>
+    <t>Archival Check</t>
+  </si>
+  <si>
+    <t>Outbound Check</t>
+  </si>
+  <si>
+    <t>BI Report Data Check</t>
+  </si>
+  <si>
+    <t>Test Execution</t>
+  </si>
+  <si>
+    <t>Data Reconciliation</t>
+  </si>
+  <si>
+    <t>Iterations for Initial &amp; Incremental</t>
+  </si>
+  <si>
+    <t>Execution Duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result Analysis </t>
+  </si>
+  <si>
+    <t>Pass/Fail Ratio</t>
+  </si>
+  <si>
+    <t>Defect Detection Ratio</t>
+  </si>
+  <si>
+    <t>Performance of BI</t>
+  </si>
+  <si>
+    <t>BI Access Privileges</t>
+  </si>
+  <si>
+    <t>Data Compliance Testing</t>
+  </si>
+  <si>
+    <t>Automation Test Execution</t>
+  </si>
+  <si>
+    <t>Automation for Test Execution</t>
+  </si>
+  <si>
+    <t>Test case Optimization</t>
+  </si>
+  <si>
+    <t>Regression Run time</t>
+  </si>
+  <si>
+    <t>Execution Efficiency</t>
+  </si>
+  <si>
+    <t>Script for Test design reduction</t>
+  </si>
+  <si>
+    <t>Data Load Pipeline Testing</t>
+  </si>
+  <si>
+    <t>Automation ROI</t>
+  </si>
+  <si>
+    <t>Test Metrics</t>
+  </si>
+  <si>
+    <t>Data completeness</t>
+  </si>
+  <si>
+    <t>Data Accuracy</t>
+  </si>
+  <si>
+    <t>Data Pipeline</t>
+  </si>
+  <si>
+    <t>Duplicate Records</t>
+  </si>
+  <si>
+    <t>Reject Records</t>
+  </si>
+  <si>
+    <t>Referential Integrity</t>
+  </si>
+  <si>
+    <t>Data Load Response Time</t>
+  </si>
+  <si>
+    <t>Production support</t>
+  </si>
+  <si>
+    <t>Prod Readiness</t>
+  </si>
+  <si>
+    <t>Data Quality Check in CICD</t>
+  </si>
+  <si>
+    <t>Data Quality Alert &amp; Notification</t>
+  </si>
+  <si>
+    <t>RCA of Prod Defect</t>
+  </si>
+  <si>
+    <t>Prod Defect Priority</t>
+  </si>
+  <si>
+    <t>Defect Occurrence ratio</t>
+  </si>
+  <si>
+    <t>Defect Retest SLA</t>
+  </si>
+  <si>
+    <t>Non-Functional Requirements</t>
+  </si>
+  <si>
+    <t>NFR Gathering and Quetionare</t>
+  </si>
+  <si>
+    <t>Performance Script/Tool Evaluation</t>
+  </si>
+  <si>
+    <t>Requirements Sign-off</t>
+  </si>
+  <si>
+    <t>Performance Test Strategy</t>
+  </si>
+  <si>
+    <t>Test plan &amp; Strategy document</t>
+  </si>
+  <si>
+    <t>Define scope of testing</t>
+  </si>
+  <si>
+    <t>SLA - Service Level Agreement</t>
+  </si>
+  <si>
+    <t>System monitoring &amp; Diagnostics tools</t>
+  </si>
+  <si>
+    <t>Workload Model</t>
+  </si>
+  <si>
+    <t>Design Scenarios</t>
+  </si>
+  <si>
+    <t>Performance Test Design</t>
+  </si>
+  <si>
+    <t>Test Environment Setup</t>
+  </si>
+  <si>
+    <t>Test Data Preparation</t>
+  </si>
+  <si>
+    <t>Test Script Design</t>
+  </si>
+  <si>
+    <t>Installation tools and configuration</t>
+  </si>
+  <si>
+    <t>Performance Test Execution</t>
+  </si>
+  <si>
+    <t>Baseline Test</t>
+  </si>
+  <si>
+    <t>Loading Test scripts</t>
+  </si>
+  <si>
+    <t>Test script execution</t>
+  </si>
+  <si>
+    <t>Monitoring execution</t>
+  </si>
+  <si>
+    <t>Collecting logs and metrics</t>
+  </si>
+  <si>
+    <t>Creation of Graphs and Charts for reports</t>
+  </si>
+  <si>
+    <t>Correlate with various charts and graphs</t>
+  </si>
+  <si>
+    <t>Detailed test report</t>
+  </si>
+  <si>
+    <t>Test report analysis and review</t>
+  </si>
+  <si>
+    <t>Defect management logger and tracking process</t>
+  </si>
+  <si>
+    <t>Tuning recommendation</t>
+  </si>
+  <si>
+    <t>Benchmark and recommendation</t>
+  </si>
+  <si>
+    <t>Comparing Load results</t>
+  </si>
+  <si>
+    <t>Validate with NFR</t>
+  </si>
+  <si>
+    <t>Test report and presentation</t>
+  </si>
+  <si>
+    <t>Performance Test  Analysis</t>
+  </si>
+  <si>
+    <t>Data TestStrategy Efficiency</t>
+  </si>
+  <si>
+    <t>DataTestPlan Efficiency</t>
+  </si>
+  <si>
+    <t>Data QualityCheck</t>
+  </si>
+  <si>
+    <t>Data PipelineCheck</t>
+  </si>
+  <si>
+    <t>Test Env Readiness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Performance Test Results </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -313,6 +624,19 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -331,16 +655,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{B3144B34-6BF3-E34F-BA27-381DD10DDB75}"/>
+    <cellStyle name="Normal 5" xfId="2" xr:uid="{53470A67-D829-044F-B1D5-2AF328ABD3D2}"/>
+    <cellStyle name="Normal 6" xfId="1" xr:uid="{8447F928-F535-834B-867F-A61E460E0F04}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1125,13 +1455,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6683460-FCD9-E649-8E4B-CD3B66BAC1EF}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="177" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="172.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1653,4 +1985,1314 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45B9211-B46E-A948-BC98-DE72E3A881E9}">
+  <dimension ref="A1:D63"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="b">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="b">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="b">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="b">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="b">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="b">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="b">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="b">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="b">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="b">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="b">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="b">
+        <v>0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="b">
+        <v>0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="b">
+        <v>0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>123</v>
+      </c>
+      <c r="D45" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="b">
+        <v>0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>123</v>
+      </c>
+      <c r="D46" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="b">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>123</v>
+      </c>
+      <c r="D47" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" t="b">
+        <v>0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" t="b">
+        <v>0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>123</v>
+      </c>
+      <c r="D49" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" t="b">
+        <v>0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>131</v>
+      </c>
+      <c r="D50" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" t="b">
+        <v>0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>131</v>
+      </c>
+      <c r="D51" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" t="b">
+        <v>0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>131</v>
+      </c>
+      <c r="D52" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" t="b">
+        <v>0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" t="b">
+        <v>0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>131</v>
+      </c>
+      <c r="D54" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" t="b">
+        <v>0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>131</v>
+      </c>
+      <c r="D55" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" t="b">
+        <v>0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>131</v>
+      </c>
+      <c r="D56" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" t="b">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>139</v>
+      </c>
+      <c r="D57" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" t="b">
+        <v>0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>139</v>
+      </c>
+      <c r="D58" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" t="b">
+        <v>0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>139</v>
+      </c>
+      <c r="D59" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60" t="b">
+        <v>0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>139</v>
+      </c>
+      <c r="D60" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61" t="b">
+        <v>0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>139</v>
+      </c>
+      <c r="D61" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62" t="b">
+        <v>0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>139</v>
+      </c>
+      <c r="D62" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63" t="b">
+        <v>0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>139</v>
+      </c>
+      <c r="D63" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FEF895C-A9B1-7D46-B818-BA918CB45A9C}">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>158</v>
+      </c>
+      <c r="D12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D19" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D20" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>185</v>
+      </c>
+      <c r="D21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>185</v>
+      </c>
+      <c r="D22" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="b">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>185</v>
+      </c>
+      <c r="D23" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>185</v>
+      </c>
+      <c r="D24" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>179</v>
+      </c>
+      <c r="D25" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="b">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>175</v>
+      </c>
+      <c r="D26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>175</v>
+      </c>
+      <c r="D27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="b">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>175</v>
+      </c>
+      <c r="D28" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
db & perf pie chart and data preview tabs
</commit_message>
<xml_diff>
--- a/data/tmm_template.xlsx
+++ b/data/tmm_template.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="98" documentId="8_{FAB75980-B740-0B40-A252-06969CBDD95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D472CE4-C284-CB47-992E-977BBCB2A2E7}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="680" windowWidth="24460" windowHeight="16940" activeTab="3" xr2:uid="{6FC6947F-CD69-5746-A992-4DF59BEE85A0}"/>
+    <workbookView xWindow="1720" yWindow="680" windowWidth="24460" windowHeight="16940" xr2:uid="{6FC6947F-CD69-5746-A992-4DF59BEE85A0}"/>
   </bookViews>
   <sheets>
     <sheet name="QA PROCESS" sheetId="1" r:id="rId1"/>
@@ -1008,7 +1008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3717E941-564B-D842-9DAF-CA0B730B6DC2}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1455,8 +1455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6683460-FCD9-E649-8E4B-CD3B66BAC1EF}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1991,9 +1991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45B9211-B46E-A948-BC98-DE72E3A881E9}">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2891,9 +2889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FEF895C-A9B1-7D46-B818-BA918CB45A9C}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>